<commit_message>
modification pour les images et le site
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeyemelodie/www/lachouetteagence/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AB95A9-46C7-1F4C-8789-32A8FE066CD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuil1" sheetId="1" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgajbA1sRpj4h647px0Becg4xhqcQ=="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Catégorie</t>
   </si>
@@ -37,36 +46,167 @@
   </si>
   <si>
     <t>(SEO ou accessiblité ?)</t>
+  </si>
+  <si>
+    <t>Format images</t>
+  </si>
+  <si>
+    <t>Images lourde</t>
+  </si>
+  <si>
+    <t>cache</t>
+  </si>
+  <si>
+    <t>texte non visible pendant le chargement</t>
+  </si>
+  <si>
+    <t>taille des images</t>
+  </si>
+  <si>
+    <t>pas de width ni de height aux images</t>
+  </si>
+  <si>
+    <t>Évitez de créer des chaînes de requêtes critiques</t>
+  </si>
+  <si>
+    <t>Réduisez au maximum le nombre de requêtes et la taille des transferts</t>
+  </si>
+  <si>
+    <t>Élément identifié comme "Largest Contentful Paint"</t>
+  </si>
+  <si>
+    <t>Éviter les changements de mise en page importants</t>
+  </si>
+  <si>
+    <t>fichier non utiliser</t>
+  </si>
+  <si>
+    <t>pas de meta description</t>
+  </si>
+  <si>
+    <t>https://web.dev/meta-description/</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>https://web.dev/lighthouse-largest-contentful-paint</t>
+  </si>
+  <si>
+    <t>https://web.dev/use-lighthouse-for-performance-budgets</t>
+  </si>
+  <si>
+    <t>https://web.dev/critical-request-chains</t>
+  </si>
+  <si>
+    <t>https://web.dev/uses-webp-images</t>
+  </si>
+  <si>
+    <t>https://web.dev/uses-optimized-images</t>
+  </si>
+  <si>
+    <t>https://web.dev/uses-responsive-images</t>
+  </si>
+  <si>
+    <t>https://web.dev/uses-long-cache-ttl</t>
+  </si>
+  <si>
+    <t>https://web.dev/optimize-cls#images-without-dimensions</t>
+  </si>
+  <si>
+    <t>https://web.dev/font-display</t>
+  </si>
+  <si>
+    <t>Les formats d'image comme JPEG 2000, JPEG XR et WebP proposent souvent une meilleure compression que les formats PNG ou JPEG. Par conséquent, les téléchargements sont plus rapides et la consommation de données est réduite.</t>
+  </si>
+  <si>
+    <t>Les images optimisées se chargent plus rapidement et consomment moins de données mobiles.</t>
+  </si>
+  <si>
+    <t>Diffusez des images de taille appropriée afin d'économiser des données mobiles et de réduire le temps de chargement.</t>
+  </si>
+  <si>
+    <t>Une longue durée de vie du cache peut accélérer les visites répétées sur votre page.</t>
+  </si>
+  <si>
+    <t>Utilisez la fonction d'affichage de la police CSS afin que le texte soit visible par l'utilisateur pendant le chargement des polices Web.</t>
+  </si>
+  <si>
+    <t>Indiquez une largeur et une hauteur explicites sur les éléments d'image afin de réduire les décalages de mise en page et d'améliorer le CLS.</t>
+  </si>
+  <si>
+    <t>Évitez d'énormes charges utiles de réseau</t>
+  </si>
+  <si>
+    <t>Les charges utiles des grands réseaux coûtent de l'argent réel aux utilisateurs et sont fortement corrélées aux délais de chargement interminables</t>
+  </si>
+  <si>
+    <t>Les chaînes de demandes critiques ci-dessous vous montrent quelles ressources sont chargées avec une priorité élevée. Envisagez de réduire la longueur des chaînes et la taille de téléchargement des ressources ou de reporter le téléchargement de ressources inutiles afin d'améliorer le chargement des pages.</t>
+  </si>
+  <si>
+    <t>Pour définir des budgets liés à la quantité et à la taille des ressources de pages, ajoutez un fichier budget.json.</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'élément identifié comme "Largest Contentful Paint" dans la fenêtre d'affichage.</t>
+  </si>
+  <si>
+    <t>Ces éléments DOM contribuent en grande partie au CLS de la page.</t>
+  </si>
+  <si>
+    <t>https://web.dev/total-byte-weight</t>
+  </si>
+  <si>
+    <t>compresser les images</t>
+  </si>
+  <si>
+    <t>accessibilité</t>
+  </si>
+  <si>
+    <t>html n'a pas de lang</t>
+  </si>
+  <si>
+    <t>https://web.dev/html-lang-valid/</t>
+  </si>
+  <si>
+    <t>il y a un fichier javascript et css non utilisé lors du chargement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -74,7 +214,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -84,43 +224,54 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -310,26 +461,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="21.33"/>
-    <col customWidth="1" min="5" max="5" width="18.78"/>
-    <col customWidth="1" min="6" max="6" width="21.33"/>
-    <col customWidth="1" min="7" max="26" width="10.56"/>
+    <col min="1" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -369,80 +522,233 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
       <c r="E2" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
       <c r="E3" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
       <c r="E4" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
       <c r="E5" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
       <c r="E6" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F6" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
       <c r="E7" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F7" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
       <c r="E8" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F8" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
       <c r="E9" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F9" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
       <c r="E10" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F10" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
       <c r="E11" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
       <c r="E12" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
       <c r="E14" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
       <c r="E15" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1428,9 +1734,14 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <hyperlinks>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{779C786A-24CE-5A43-9DF4-03BDC7BE0D0A}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{C682C391-2110-874D-8739-C4E11BE03469}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{CE919627-9D05-D04E-B7B4-326D2E89DB49}"/>
+    <hyperlink ref="F7" r:id="rId4" location="images-without-dimensions" display="https://web.dev/optimize-cls/?utm_source=lighthouse&amp;utm_medium=unknown#images-without-dimensions" xr:uid="{79124408-7D43-B049-B338-AFE7D0B1E524}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{0F13B5D3-2A4C-7D4A-89E3-B185D2FD3E3D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout fichier pour sitemap
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeyemelodie/www/lachouetteagence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9996220F-C574-3F42-A405-C890C9FCE934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC42A78-37BC-C54E-9454-3DEC1BF7CD0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32680" yWindow="-420" windowWidth="22980" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="22980" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>

</xml_diff>